<commit_message>
Many changes, among them, replacing the Composite out with SCART-rgb.
</commit_message>
<xml_diff>
--- a/Docs/Changelog.xlsx
+++ b/Docs/Changelog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Teknikprojekt\Hardware\MSX\trh9000\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68762478-0B9B-4401-B937-D00DFA84F4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAD0E0A-1676-42AC-AD0E-9A8D0E2871F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -33,14 +33,48 @@
     <t>Note</t>
   </si>
   <si>
-    <t>Added a changelog-file, altered the .gitignore according to the Kicad standard, started adding annotations to the datasheets for navigation</t>
+    <t>Contributor</t>
+  </si>
+  <si>
+    <t>Added a changelog-file, 
+altered the .gitignore according to 
+the Kicad standard, started adding 
+annotations to the datasheets for navigation.</t>
+  </si>
+  <si>
+    <t>Doomn00b</t>
+  </si>
+  <si>
+    <t>Changed the project to use generic
+links instead of local links, merged footprint
+libraries into one, merged symbol libraries into one,
+started rewriting V9990 datasheet with Open Sans font,
+for future open source datasheet</t>
+  </si>
+  <si>
+    <t>Changed V9990 symbol and footprint</t>
+  </si>
+  <si>
+    <t>Replaced C3 THT capacitor with SMD.</t>
+  </si>
+  <si>
+    <t>Replaced RGB-connector with real VGA conn from Amphenol, changed decoupling, put power-parts on their own sheet,</t>
+  </si>
+  <si>
+    <t>Replaced big 14MHz oscillator with SMD one,</t>
+  </si>
+  <si>
+    <t>Changed the glue logic to use Advanced 74xx versions, with far higher performance.</t>
+  </si>
+  <si>
+    <t>Removed Composite video and replaced with RGB Scart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,8 +90,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,8 +130,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -136,19 +183,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -427,86 +495,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44778</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="5"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44784</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="5"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>44785</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="5"/>
     </row>

</xml_diff>

<commit_message>
Multiple updates. Routing. Almost finished routing for the VDP. Moved back the footprint for the 14mhz oscillator to THT as it is easier to find outside US/Europe and I have a bunch laying around here. Organized all components into the PCB. Removed the holed in the cartridge so I can better measure them in the standard MSX cartridge. Changed the RGB connector footprint to a shorter version so we can fit it in the standard size cartridge. Fixed multiple footprints to 0805 as we will be standardizing in that size.
</commit_message>
<xml_diff>
--- a/Docs/Changelog.xlsx
+++ b/Docs/Changelog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Teknikprojekt\Hardware\MSX\trh9000\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70c233ac39d07974/Personal/11. Electronics/V9990/trh9000/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAD0E0A-1676-42AC-AD0E-9A8D0E2871F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{9AAD0E0A-1676-42AC-AD0E-9A8D0E2871F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60BA8C27-F525-497C-9B92-E29F916DB05C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Removed Composite video and replaced with RGB Scart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Routing. Almost finished routing for the VDP. Moved back the footprint for the 14mhz oscillator to THT as it is easier to find outside US/Europe and I have a bunch laying around here. Organized all components into the PCB. Removed the holed in the cartridge so I can better measure them in the standard MSX cartridge. Changed the RGB connector footprint to a shorter version so we can fit it in the standard size cartridge. Fixed multiple footprints to 0805 as we will be standardizing in that size. </t>
   </si>
 </sst>
 </file>
@@ -203,17 +206,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -498,13 +502,13 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="156.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -512,29 +516,29 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44778</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44784</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
@@ -543,13 +547,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -557,67 +561,71 @@
       <c r="A6" s="2">
         <v>44785</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5"/>
+    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>44793</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="5"/>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="5"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="5"/>
+      <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="5"/>
+      <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="5"/>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="5"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="5"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="5"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="5"/>
+      <c r="B19" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>